<commit_message>
1. Corrected the input file 2. Added output file 3. Add the binary file
</commit_message>
<xml_diff>
--- a/Simplify/Release/V1.0.0.0/JournalFY17.xlsx
+++ b/Simplify/Release/V1.0.0.0/JournalFY17.xlsx
@@ -474,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -789,7 +789,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3">
         <v>42744</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3">
         <v>42744</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3">
         <v>42745</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3">
         <v>42745</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3">
         <v>42771</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3">
         <v>42771</v>
@@ -905,7 +905,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3">
         <v>42776</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3">
         <v>42776</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3">
         <v>42797</v>
@@ -963,7 +963,7 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3">
         <v>42797</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3">
         <v>42819</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3">
         <v>42819</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3">
         <v>42819</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3">
         <v>42825</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3">
         <v>42825</v>
@@ -1081,9 +1081,6 @@
       <c r="F30" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="C31" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F30">

</xml_diff>